<commit_message>
Biweekly meeting, BEGUN Bauteilevaluation
</commit_message>
<xml_diff>
--- a/diagramme/Leistungsbudget.xlsx
+++ b/diagramme/Leistungsbudget.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\Studium\Juventus\Diplomarbeit\Nathophone_doc\diagramme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37911681-927F-44E9-808E-11DCEB5344B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9AA2B0-E7AD-48AD-8835-4C81567D45B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DF0AED17-E800-4598-8D02-E0D18B4072C0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DF0AED17-E800-4598-8D02-E0D18B4072C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -141,10 +142,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -197,7 +198,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -210,7 +211,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-CH" sz="2000">
+              <a:rPr lang="de-CH" sz="1800">
                 <a:latin typeface="Fira Sans SemiBold" panose="020B0603050000020004" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t>Leistungsbudget</a:t>
@@ -231,7 +232,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -361,13 +362,209 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-92F7-4F56-8F83-A7A96BC38BF4}"/>
+              <c16:uniqueId val="{00000000-71BA-474C-8398-55D12913724E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Endstufe: Minimum pro Kanal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F24444"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Fira Sans" panose="020B0503050000020004" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-71BA-474C-8398-55D12913724E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Endstufe: Empfohlen pro Kanal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="AD0B0B"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Fira Sans" panose="020B0503050000020004" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-71BA-474C-8398-55D12913724E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$A$5</c:f>
@@ -462,13 +659,13 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-92F7-4F56-8F83-A7A96BC38BF4}"/>
+              <c16:uniqueId val="{00000003-71BA-474C-8398-55D12913724E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$A$7</c:f>
@@ -560,13 +757,13 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-92F7-4F56-8F83-A7A96BC38BF4}"/>
+              <c16:uniqueId val="{00000004-71BA-474C-8398-55D12913724E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$A$8</c:f>
@@ -658,203 +855,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-92F7-4F56-8F83-A7A96BC38BF4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Endstufe: Minimum pro Kanal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="F24444"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Fira Sans" panose="020B0503050000020004" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>7.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-92F7-4F56-8F83-A7A96BC38BF4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Endstufe: Empfohlen pro Kanal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="AD0B0B"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Fira Sans" panose="020B0503050000020004" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-92F7-4F56-8F83-A7A96BC38BF4}"/>
+              <c16:uniqueId val="{00000005-71BA-474C-8398-55D12913724E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -952,7 +953,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-92F7-4F56-8F83-A7A96BC38BF4}"/>
+              <c16:uniqueId val="{00000006-71BA-474C-8398-55D12913724E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1050,7 +1051,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-92F7-4F56-8F83-A7A96BC38BF4}"/>
+              <c16:uniqueId val="{00000007-71BA-474C-8398-55D12913724E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1148,7 +1149,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-92F7-4F56-8F83-A7A96BC38BF4}"/>
+              <c16:uniqueId val="{00000008-71BA-474C-8398-55D12913724E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1246,7 +1247,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-92F7-4F56-8F83-A7A96BC38BF4}"/>
+              <c16:uniqueId val="{00000009-71BA-474C-8398-55D12913724E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1344,7 +1345,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-92F7-4F56-8F83-A7A96BC38BF4}"/>
+              <c16:uniqueId val="{0000000A-71BA-474C-8398-55D12913724E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1442,7 +1443,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-92F7-4F56-8F83-A7A96BC38BF4}"/>
+              <c16:uniqueId val="{0000000B-71BA-474C-8398-55D12913724E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1519,7 +1520,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1532,7 +1533,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-CH"/>
+                  <a:rPr lang="de-CH" sz="1600"/>
                   <a:t>Nennleistung in [Watt]</a:t>
                 </a:r>
               </a:p>
@@ -1551,7 +1552,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1583,7 +1584,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1616,10 +1617,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66062037944181706"/>
-          <c:y val="2.9442174853666306E-2"/>
-          <c:w val="0.3291389651562372"/>
-          <c:h val="0.9705578251463336"/>
+          <c:x val="0.68806551961478879"/>
+          <c:y val="1.2501698862173628E-2"/>
+          <c:w val="0.30169385305197172"/>
+          <c:h val="0.98749830113782633"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1635,7 +1636,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2244,27 +2245,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>886691</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>166254</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>96981</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8951DDA5-687F-1194-956B-E387414A27AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADA7C641-2B38-47D4-B556-7743FD2DDEC5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2600,8 +2603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7534DA1-B209-43BD-886F-D59B11C48C35}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2621,11 +2624,11 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
@@ -2659,11 +2662,11 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
@@ -2688,7 +2691,7 @@
       <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
@@ -2715,11 +2718,11 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
@@ -2746,11 +2749,11 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
@@ -2805,6 +2808,21 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CE5BDB-7762-4715-AFC7-FB3FAF48000F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>